<commit_message>
Update code with user management for access token
</commit_message>
<xml_diff>
--- a/IndustryProjectData/Food Data.xlsx
+++ b/IndustryProjectData/Food Data.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Lor Mee</t>
   </si>
   <si>
-    <t xml:space="preserve">Minced port Noodle - Dry</t>
+    <t xml:space="preserve">Minced Pork Noodle - Dry</t>
   </si>
   <si>
     <t xml:space="preserve">Minced Pork Noodle - Soup</t>
@@ -352,12 +352,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -394,8 +400,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -488,13 +498,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L80"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="86:86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -550,7 +560,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -568,10 +578,10 @@
       <c r="F4" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>3.8</v>
       </c>
       <c r="I4" s="0" t="n">
@@ -580,15 +590,15 @@
       <c r="J4" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="2" t="n">
         <v>73</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="2" t="n">
         <v>486</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <f aca="false">A4+1</f>
         <v>2</v>
       </c>
@@ -607,10 +617,10 @@
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="I5" s="0" t="n">
@@ -619,15 +629,15 @@
       <c r="J5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="K5" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="2" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <f aca="false">A5+1</f>
         <v>3</v>
       </c>
@@ -646,10 +656,10 @@
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="2" t="n">
         <v>0.4</v>
       </c>
       <c r="I6" s="0" t="n">
@@ -658,15 +668,15 @@
       <c r="J6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="K6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="L6" s="2" t="n">
         <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <f aca="false">A6+1</f>
         <v>4</v>
       </c>
@@ -685,10 +695,10 @@
       <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="2" t="n">
         <v>1.7</v>
       </c>
       <c r="I7" s="0" t="n">
@@ -697,15 +707,15 @@
       <c r="J7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="K7" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="L7" s="2" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="1" t="n">
         <f aca="false">A7+1</f>
         <v>5</v>
       </c>
@@ -724,10 +734,10 @@
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="2" t="n">
         <v>1.5</v>
       </c>
       <c r="I8" s="0" t="n">
@@ -736,15 +746,15 @@
       <c r="J8" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="K8" s="2" t="n">
+      <c r="K8" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="L8" s="2" t="n">
+      <c r="L8" s="3" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <f aca="false">A8+1</f>
         <v>6</v>
       </c>
@@ -763,10 +773,10 @@
       <c r="F9" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="2" t="n">
         <v>8.4</v>
       </c>
       <c r="I9" s="0" t="n">
@@ -775,10 +785,10 @@
       <c r="J9" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="K9" s="1" t="n">
+      <c r="K9" s="2" t="n">
         <v>232</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="L9" s="2" t="n">
         <v>2196</v>
       </c>
     </row>
@@ -802,10 +812,10 @@
       <c r="F10" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="2" t="n">
         <v>29.2</v>
       </c>
       <c r="I10" s="0" t="n">
@@ -814,10 +824,10 @@
       <c r="J10" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="K10" s="1" t="n">
+      <c r="K10" s="2" t="n">
         <v>234</v>
       </c>
-      <c r="L10" s="1" t="n">
+      <c r="L10" s="2" t="n">
         <v>1459</v>
       </c>
     </row>
@@ -841,10 +851,10 @@
       <c r="F11" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="2" t="n">
         <v>11.9</v>
       </c>
       <c r="I11" s="0" t="n">
@@ -853,10 +863,10 @@
       <c r="J11" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="K11" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="L11" s="1" t="n">
+      <c r="L11" s="2" t="n">
         <v>880</v>
       </c>
     </row>
@@ -880,10 +890,10 @@
       <c r="F12" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="G12" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="2" t="n">
         <v>8.7</v>
       </c>
       <c r="I12" s="0" t="n">
@@ -892,10 +902,10 @@
       <c r="J12" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="K12" s="2" t="n">
+      <c r="K12" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="L12" s="2" t="n">
         <v>1287</v>
       </c>
     </row>
@@ -919,10 +929,10 @@
       <c r="F13" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H13" s="2" t="n">
+      <c r="H13" s="3" t="n">
         <v>1.8</v>
       </c>
       <c r="I13" s="0" t="n">
@@ -931,10 +941,10 @@
       <c r="J13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="K13" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="L13" s="2" t="n">
         <v>909</v>
       </c>
     </row>
@@ -958,10 +968,10 @@
       <c r="F14" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="2" t="n">
         <v>5.9</v>
       </c>
       <c r="I14" s="0" t="n">
@@ -970,10 +980,10 @@
       <c r="J14" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="K14" s="2" t="n">
         <v>92</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="L14" s="2" t="n">
         <v>545</v>
       </c>
     </row>
@@ -997,10 +1007,10 @@
       <c r="F15" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="H15" s="2" t="n">
+      <c r="H15" s="3" t="n">
         <v>3.6</v>
       </c>
       <c r="I15" s="0" t="n">
@@ -1009,10 +1019,10 @@
       <c r="J15" s="0" t="n">
         <v>99</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="K15" s="2" t="n">
         <v>80</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="L15" s="3" t="n">
         <v>326</v>
       </c>
     </row>
@@ -1036,10 +1046,10 @@
       <c r="F16" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H16" s="2" t="n">
+      <c r="H16" s="3" t="n">
         <v>3.3</v>
       </c>
       <c r="I16" s="0" t="n">
@@ -1048,10 +1058,10 @@
       <c r="J16" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K16" s="2" t="n">
+      <c r="K16" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="L16" s="1" t="n">
+      <c r="L16" s="2" t="n">
         <v>1645</v>
       </c>
     </row>
@@ -1075,10 +1085,10 @@
       <c r="F17" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H17" s="2" t="n">
+      <c r="H17" s="3" t="n">
         <v>2.4</v>
       </c>
       <c r="I17" s="0" t="n">
@@ -1087,10 +1097,10 @@
       <c r="J17" s="0" t="n">
         <v>88</v>
       </c>
-      <c r="K17" s="2" t="n">
+      <c r="K17" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="L17" s="1" t="n">
+      <c r="L17" s="2" t="n">
         <v>2913</v>
       </c>
     </row>
@@ -1114,10 +1124,10 @@
       <c r="F18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="G18" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="H18" s="1" t="n">
+      <c r="H18" s="2" t="n">
         <v>14.1</v>
       </c>
       <c r="I18" s="0" t="n">
@@ -1126,10 +1136,10 @@
       <c r="J18" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="K18" s="1" t="n">
+      <c r="K18" s="2" t="n">
         <v>109</v>
       </c>
-      <c r="L18" s="1" t="n">
+      <c r="L18" s="2" t="n">
         <v>1289</v>
       </c>
     </row>
@@ -1153,10 +1163,10 @@
       <c r="F19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="G19" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="2" t="n">
         <v>7.3</v>
       </c>
       <c r="I19" s="0" t="n">
@@ -1165,10 +1175,10 @@
       <c r="J19" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="K19" s="1" t="n">
+      <c r="K19" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="L19" s="1" t="n">
+      <c r="L19" s="2" t="n">
         <v>1423</v>
       </c>
     </row>
@@ -1192,10 +1202,10 @@
       <c r="F20" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="2" t="n">
         <v>13.6</v>
       </c>
       <c r="I20" s="0" t="n">
@@ -1204,10 +1214,10 @@
       <c r="J20" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="K20" s="1" t="n">
+      <c r="K20" s="2" t="n">
         <v>175</v>
       </c>
-      <c r="L20" s="1" t="n">
+      <c r="L20" s="2" t="n">
         <v>1245</v>
       </c>
     </row>
@@ -1231,10 +1241,10 @@
       <c r="F21" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="G21" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="H21" s="1" t="n">
+      <c r="H21" s="2" t="n">
         <v>11.6</v>
       </c>
       <c r="I21" s="0" t="n">
@@ -1243,10 +1253,10 @@
       <c r="J21" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="K21" s="1" t="n">
+      <c r="K21" s="2" t="n">
         <v>348</v>
       </c>
-      <c r="L21" s="1" t="n">
+      <c r="L21" s="2" t="n">
         <v>2303</v>
       </c>
     </row>
@@ -1270,10 +1280,10 @@
       <c r="F22" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="G22" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="H22" s="1" t="n">
+      <c r="H22" s="2" t="n">
         <v>17.8</v>
       </c>
       <c r="I22" s="0" t="n">
@@ -1282,10 +1292,10 @@
       <c r="J22" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="K22" s="1" t="n">
+      <c r="K22" s="2" t="n">
         <v>81</v>
       </c>
-      <c r="L22" s="1" t="n">
+      <c r="L22" s="2" t="n">
         <v>1588</v>
       </c>
     </row>
@@ -1309,10 +1319,10 @@
       <c r="F23" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="H23" s="2" t="n">
+      <c r="H23" s="3" t="n">
         <v>4.9</v>
       </c>
       <c r="I23" s="0" t="n">
@@ -1321,10 +1331,10 @@
       <c r="J23" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="K23" s="2" t="n">
         <v>140</v>
       </c>
-      <c r="L23" s="1" t="n">
+      <c r="L23" s="2" t="n">
         <v>2538</v>
       </c>
     </row>
@@ -1348,10 +1358,10 @@
       <c r="F24" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="G24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="2" t="n">
         <v>9.2</v>
       </c>
       <c r="I24" s="0" t="n">
@@ -1360,10 +1370,10 @@
       <c r="J24" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="K24" s="2" t="n">
+      <c r="K24" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="L24" s="1" t="n">
+      <c r="L24" s="2" t="n">
         <v>1491</v>
       </c>
     </row>
@@ -1387,10 +1397,10 @@
       <c r="F25" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="H25" s="2" t="n">
+      <c r="H25" s="3" t="n">
         <v>4.8</v>
       </c>
       <c r="I25" s="0" t="n">
@@ -1399,10 +1409,10 @@
       <c r="J25" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="K25" s="2" t="n">
+      <c r="K25" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="L25" s="1" t="n">
+      <c r="L25" s="2" t="n">
         <v>1740</v>
       </c>
     </row>
@@ -1426,10 +1436,10 @@
       <c r="F26" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H26" s="2" t="n">
+      <c r="H26" s="3" t="n">
         <v>0.6</v>
       </c>
       <c r="I26" s="0" t="n">
@@ -1438,10 +1448,10 @@
       <c r="J26" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="K26" s="2" t="n">
+      <c r="K26" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="L26" s="1" t="n">
+      <c r="L26" s="2" t="n">
         <v>2287</v>
       </c>
     </row>
@@ -1465,10 +1475,10 @@
       <c r="F27" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H27" s="2" t="n">
+      <c r="H27" s="3" t="n">
         <v>2.3</v>
       </c>
       <c r="I27" s="0" t="n">
@@ -1477,10 +1487,10 @@
       <c r="J27" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="K27" s="1" t="n">
+      <c r="K27" s="2" t="n">
         <v>370</v>
       </c>
-      <c r="L27" s="1" t="n">
+      <c r="L27" s="2" t="n">
         <v>834</v>
       </c>
     </row>
@@ -1504,10 +1514,10 @@
       <c r="F28" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="G28" s="2" t="n">
+      <c r="G28" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="H28" s="2" t="n">
+      <c r="H28" s="3" t="n">
         <v>1.1</v>
       </c>
       <c r="I28" s="0" t="n">
@@ -1516,10 +1526,10 @@
       <c r="J28" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="K28" s="2" t="n">
+      <c r="K28" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="L28" s="1" t="n">
+      <c r="L28" s="2" t="n">
         <v>2422</v>
       </c>
     </row>
@@ -1543,22 +1553,22 @@
       <c r="F29" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="H29" s="2" t="n">
+      <c r="H29" s="3" t="n">
         <v>3.5</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>3.4</v>
       </c>
-      <c r="J29" s="3" t="n">
+      <c r="J29" s="4" t="n">
         <v>48</v>
       </c>
-      <c r="K29" s="2" t="n">
+      <c r="K29" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="L29" s="1" t="n">
+      <c r="L29" s="2" t="n">
         <v>1413</v>
       </c>
     </row>
@@ -1582,10 +1592,10 @@
       <c r="F30" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="H30" s="2" t="n">
+      <c r="H30" s="3" t="n">
         <v>5</v>
       </c>
       <c r="I30" s="0" t="n">
@@ -1594,10 +1604,10 @@
       <c r="J30" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="K30" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="L30" s="1" t="n">
+      <c r="L30" s="2" t="n">
         <v>1502</v>
       </c>
     </row>
@@ -1621,10 +1631,10 @@
       <c r="F31" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G31" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="H31" s="2" t="n">
+      <c r="H31" s="3" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="0" t="n">
@@ -1633,1520 +1643,1319 @@
       <c r="J31" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="K31" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="L31" s="1" t="n">
+      <c r="L31" s="2" t="n">
         <v>1804</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <f aca="false">A31+1</f>
-        <v>29</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="0" t="n">
-        <v>210</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>494</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="K32" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="L32" s="1" t="n">
-        <v>838</v>
-      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <f aca="false">A32+1</f>
-        <v>30</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="0" t="n">
-        <v>920</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>359</v>
-      </c>
-      <c r="F33" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="H33" s="1" t="n">
-        <v>6.8</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="K33" s="2" t="n">
-        <v>62</v>
-      </c>
-      <c r="L33" s="1" t="n">
-        <v>1537</v>
-      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <f aca="false">A33+1</f>
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>775</v>
+        <v>210</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>798</v>
+        <v>494</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="H34" s="1" t="n">
-        <v>21.9</v>
+        <v>13</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>7.6</v>
       </c>
       <c r="I34" s="0" t="n">
-        <v>13.2</v>
+        <v>6.5</v>
       </c>
       <c r="J34" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="K34" s="1" t="n">
-        <v>264</v>
-      </c>
-      <c r="L34" s="1" t="n">
-        <v>1930</v>
+        <v>80</v>
+      </c>
+      <c r="K34" s="2" t="n">
+        <v>76</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>838</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <f aca="false">A34+1</f>
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>571</v>
+        <v>920</v>
       </c>
       <c r="E35" s="0" t="n">
-        <v>571</v>
+        <v>359</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G35" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="H35" s="1" t="n">
-        <v>5.8</v>
+      <c r="H35" s="2" t="n">
+        <v>6.8</v>
       </c>
       <c r="I35" s="0" t="n">
-        <v>8</v>
+        <v>3.5</v>
       </c>
       <c r="J35" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="K35" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="L35" s="1" t="n">
-        <v>2164</v>
+        <v>31</v>
+      </c>
+      <c r="K35" s="3" t="n">
+        <v>62</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>1537</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <f aca="false">A35+1</f>
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" s="0" t="n">
-        <v>541</v>
+        <v>775</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>433</v>
+        <v>798</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="H36" s="1" t="n">
-        <v>5.4</v>
+        <v>46</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <v>40</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>21.9</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>3.8</v>
+        <v>13.2</v>
       </c>
       <c r="J36" s="0" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K36" s="2" t="n">
-        <v>38</v>
-      </c>
-      <c r="L36" s="1" t="n">
-        <v>2678</v>
+        <v>264</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>1930</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <f aca="false">A36+1</f>
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>37</v>
+        <v>571</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>131</v>
+        <v>571</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G37" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="I37" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="H37" s="1" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>0.6</v>
-      </c>
       <c r="J37" s="0" t="n">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="K37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" s="1" t="n">
-        <v>168</v>
+        <v>206</v>
+      </c>
+      <c r="L37" s="2" t="n">
+        <v>2164</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <f aca="false">A37+1</f>
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>65</v>
+        <v>541</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>197</v>
+        <v>433</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H38" s="1" t="n">
-        <v>3.4</v>
+        <v>19</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>5.4</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>2.3</v>
+        <v>3.8</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="K38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" s="1" t="n">
-        <v>103</v>
+        <v>60</v>
+      </c>
+      <c r="K38" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="L38" s="2" t="n">
+        <v>2678</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <f aca="false">A38+1</f>
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>488</v>
+        <v>37</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>877</v>
+        <v>131</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>14.8</v>
+        <v>4</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>3.8</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>8.4</v>
+        <v>0.6</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>102</v>
-      </c>
-      <c r="K39" s="1" t="n">
-        <v>158</v>
-      </c>
-      <c r="L39" s="1" t="n">
-        <v>1656</v>
+        <v>11</v>
+      </c>
+      <c r="K39" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="2" t="n">
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <f aca="false">A39+1</f>
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="H40" s="1" t="n">
-        <v>5.8</v>
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>3.4</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K40" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="L40" s="1" t="n">
-        <v>466</v>
+        <v>36</v>
+      </c>
+      <c r="K40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>103</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <f aca="false">A40+1</f>
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>80</v>
+        <v>488</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>141</v>
+        <v>877</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="G41" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="H41" s="1" t="n">
-        <v>3.1</v>
+        <v>39</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>14.8</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>0</v>
+        <v>8.4</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="L41" s="1" t="n">
-        <v>228</v>
+        <v>102</v>
+      </c>
+      <c r="K41" s="2" t="n">
+        <v>158</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>1656</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <f aca="false">A41+1</f>
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>377</v>
+        <v>93</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>742</v>
+        <v>208</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="G42" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="H42" s="1" t="n">
-        <v>11.3</v>
+        <v>24</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>5.8</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>4.1</v>
+        <v>2.6</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>103</v>
-      </c>
-      <c r="K42" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="L42" s="1" t="n">
-        <v>1467</v>
+        <v>1</v>
+      </c>
+      <c r="K42" s="2" t="n">
+        <v>83</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>466</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <f aca="false">A42+1</f>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>309</v>
+        <v>80</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>500</v>
+        <v>141</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="G43" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="H43" s="1" t="n">
-        <v>8.3</v>
+        <v>16</v>
+      </c>
+      <c r="G43" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>3.1</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="K43" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="L43" s="1" t="n">
-        <v>1851</v>
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="L43" s="2" t="n">
+        <v>228</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <f aca="false">A43+1</f>
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>11</v>
+        <v>377</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>31</v>
+        <v>742</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G44" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>0.6</v>
+        <v>21</v>
+      </c>
+      <c r="G44" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>11.3</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>0</v>
+        <v>4.1</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K44" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="L44" s="0" t="n">
-        <v>32</v>
+        <v>103</v>
+      </c>
+      <c r="K44" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="L44" s="2" t="n">
+        <v>1467</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <f aca="false">A44+1</f>
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>342</v>
+        <v>500</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="G45" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="H45" s="1" t="n">
-        <v>15.1</v>
+        <v>18</v>
+      </c>
+      <c r="G45" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>8.3</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>1.4</v>
+        <v>4.4</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K45" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="L45" s="1" t="n">
-        <v>480</v>
+        <v>61</v>
+      </c>
+      <c r="K45" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="L45" s="2" t="n">
+        <v>1851</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <f aca="false">A45+1</f>
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G46" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="H46" s="1" t="n">
-        <v>2.9</v>
+        <v>3</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>0.6</v>
       </c>
       <c r="I46" s="0" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="J46" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L46" s="0" t="n">
         <v>32</v>
-      </c>
-      <c r="K46" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L46" s="1" t="n">
-        <v>386</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <f aca="false">A46+1</f>
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>60</v>
+        <v>293</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>187</v>
+        <v>342</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="G47" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="H47" s="1" t="n">
-        <v>3.1</v>
+        <v>28</v>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>15.1</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>4.1</v>
+        <v>1.4</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="K47" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="K47" s="2" t="n">
+        <v>83</v>
       </c>
       <c r="L47" s="2" t="n">
-        <v>155</v>
+        <v>480</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <f aca="false">A47+1</f>
-        <v>45</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>253</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>721</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="G48" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="H48" s="1" t="n">
-        <v>18.1</v>
-      </c>
-      <c r="I48" s="0" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="J48" s="0" t="n">
-        <v>77</v>
-      </c>
-      <c r="K48" s="1" t="n">
-        <v>242</v>
-      </c>
-      <c r="L48" s="1" t="n">
-        <v>2011</v>
-      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <f aca="false">A48+1</f>
-        <v>46</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="0" t="n">
-        <v>131</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>357</v>
-      </c>
-      <c r="F49" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="H49" s="1" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="I49" s="0" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="J49" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="K49" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="L49" s="1" t="n">
-        <v>430</v>
-      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <f aca="false">A49+1</f>
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>211</v>
+        <v>70</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>373</v>
+        <v>209</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G50" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="H50" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G50" s="3" t="n">
         <v>7</v>
       </c>
+      <c r="H50" s="2" t="n">
+        <v>2.9</v>
+      </c>
       <c r="I50" s="0" t="n">
-        <v>9.3</v>
+        <v>1.7</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="K50" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="L50" s="1" t="n">
-        <v>1365</v>
+        <v>32</v>
+      </c>
+      <c r="K50" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" s="2" t="n">
+        <v>386</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <f aca="false">A50+1</f>
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="G51" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="H51" s="1" t="n">
-        <v>2.7</v>
+        <v>4</v>
+      </c>
+      <c r="G51" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>3.1</v>
       </c>
       <c r="I51" s="0" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="K51" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J51" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="K51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="L51" s="1" t="n">
-        <v>480</v>
+      <c r="L51" s="3" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <f aca="false">A51+1</f>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D52" s="0" t="n">
-        <v>455</v>
+        <v>253</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>860</v>
+        <v>721</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="G52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H52" s="1" t="n">
-        <v>18.7</v>
+        <v>25</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>18.1</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>0</v>
+        <v>11.3</v>
       </c>
       <c r="J52" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="K52" s="1" t="n">
-        <v>255</v>
-      </c>
-      <c r="L52" s="1" t="n">
-        <v>2330</v>
+        <v>77</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>242</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>2011</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <f aca="false">A52+1</f>
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>173</v>
+        <v>357</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="G53" s="2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H53" s="2" t="n">
-        <v>2.6</v>
+        <v>4.2</v>
       </c>
       <c r="I53" s="0" t="n">
-        <v>0.9</v>
+        <v>3.3</v>
       </c>
       <c r="J53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K53" s="1" t="n">
-        <v>60</v>
+        <v>57</v>
+      </c>
+      <c r="K53" s="3" t="n">
+        <v>21</v>
       </c>
       <c r="L53" s="2" t="n">
-        <v>187</v>
+        <v>430</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <f aca="false">A53+1</f>
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>934</v>
+        <v>211</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>211</v>
+        <v>373</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G54" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="H54" s="1" t="n">
-        <v>3.2</v>
+        <v>17</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>7</v>
       </c>
       <c r="I54" s="0" t="n">
-        <v>6.3</v>
+        <v>9.3</v>
       </c>
       <c r="J54" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="K54" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="L54" s="1" t="n">
-        <v>1658</v>
+      <c r="K54" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>1365</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <f aca="false">A54+1</f>
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>191</v>
+        <v>112</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>284</v>
+        <v>156</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="G55" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="H55" s="1" t="n">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="G55" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>2.7</v>
       </c>
       <c r="I55" s="0" t="n">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K55" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="L55" s="1" t="n">
-        <v>636</v>
+        <v>2</v>
+      </c>
+      <c r="K55" s="2" t="n">
+        <v>49</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <v>480</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <f aca="false">A55+1</f>
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>99</v>
+        <v>455</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>128</v>
+        <v>860</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="G56" s="2" t="n">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="H56" s="2" t="n">
-        <v>1.3</v>
+        <v>18.7</v>
       </c>
       <c r="I56" s="0" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="J56" s="0" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K56" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="L56" s="1" t="n">
-        <v>414</v>
+        <v>255</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>2330</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <f aca="false">A56+1</f>
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>859</v>
+        <v>71</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>1142</v>
+        <v>173</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="G57" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="H57" s="1" t="n">
-        <v>24.9</v>
+        <v>24</v>
+      </c>
+      <c r="G57" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>2.6</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>17.2</v>
+        <v>0.9</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>135</v>
-      </c>
-      <c r="K57" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="L57" s="1" t="n">
-        <v>1400</v>
+        <v>1</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>187</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <f aca="false">A57+1</f>
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>116</v>
+        <v>934</v>
       </c>
       <c r="E58" s="0" t="n">
-        <v>299</v>
+        <v>211</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="G58" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="H58" s="1" t="n">
-        <v>7.7</v>
+        <v>20</v>
+      </c>
+      <c r="G58" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>3.2</v>
       </c>
       <c r="I58" s="0" t="n">
-        <v>2.7</v>
+        <v>6.3</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="K58" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="L58" s="1" t="n">
-        <v>292</v>
+        <v>13</v>
+      </c>
+      <c r="K58" s="2" t="n">
+        <v>39</v>
+      </c>
+      <c r="L58" s="2" t="n">
+        <v>1658</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <f aca="false">A58+1</f>
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="E59" s="0" t="n">
-        <v>206</v>
+        <v>284</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="H59" s="1" t="n">
-        <v>5.3</v>
+        <v>34</v>
+      </c>
+      <c r="G59" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>6</v>
       </c>
       <c r="I59" s="0" t="n">
-        <v>1.8</v>
+        <v>3.3</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="K59" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="L59" s="1" t="n">
-        <v>311</v>
+        <v>146</v>
+      </c>
+      <c r="L59" s="2" t="n">
+        <v>636</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <f aca="false">A59+1</f>
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D60" s="0" t="n">
-        <v>253</v>
+        <v>99</v>
       </c>
       <c r="E60" s="0" t="n">
-        <v>305</v>
+        <v>128</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="G60" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="H60" s="1" t="n">
-        <v>8.1</v>
+        <v>23</v>
+      </c>
+      <c r="G60" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>1.3</v>
       </c>
       <c r="I60" s="0" t="n">
-        <v>15.3</v>
+        <v>0.4</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="K60" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="L60" s="1" t="n">
-        <v>1206</v>
+        <v>1</v>
+      </c>
+      <c r="K60" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="L60" s="2" t="n">
+        <v>414</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <f aca="false">A60+1</f>
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>266</v>
+        <v>859</v>
       </c>
       <c r="E61" s="0" t="n">
-        <v>516</v>
+        <v>1142</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="G61" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="H61" s="0" t="n">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="G61" s="2" t="n">
+        <v>46</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>24.9</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>5</v>
+        <v>17.2</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="K61" s="0" t="n">
-        <v>417</v>
-      </c>
-      <c r="L61" s="0" t="n">
-        <v>970</v>
+        <v>135</v>
+      </c>
+      <c r="K61" s="2" t="n">
+        <v>180</v>
+      </c>
+      <c r="L61" s="2" t="n">
+        <v>1400</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <f aca="false">A61+1</f>
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="E62" s="0" t="n">
-        <v>387</v>
+        <v>299</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="G62" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="G62" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="H62" s="0" t="n">
-        <v>5</v>
+      <c r="H62" s="2" t="n">
+        <v>7.7</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="J62" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="K62" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="L62" s="0" t="n">
-        <v>770</v>
+        <v>25</v>
+      </c>
+      <c r="K62" s="2" t="n">
+        <v>86</v>
+      </c>
+      <c r="L62" s="2" t="n">
+        <v>292</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <f aca="false">A62+1</f>
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="E63" s="0" t="n">
-        <v>332</v>
+        <v>206</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="G63" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="H63" s="0" t="n">
-        <v>3.5</v>
+        <v>4</v>
+      </c>
+      <c r="G63" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>5.3</v>
       </c>
       <c r="I63" s="0" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="K63" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L63" s="0" t="n">
-        <v>570</v>
+        <v>22</v>
+      </c>
+      <c r="K63" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L63" s="2" t="n">
+        <v>311</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <f aca="false">A63+1</f>
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>164</v>
+        <v>253</v>
       </c>
       <c r="E64" s="0" t="n">
-        <v>440</v>
+        <v>305</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="G64" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="H64" s="0" t="n">
-        <v>11.6</v>
+        <v>18</v>
+      </c>
+      <c r="G64" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>8.1</v>
       </c>
       <c r="I64" s="0" t="n">
-        <v>2</v>
+        <v>15.3</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="K64" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L64" s="0" t="n">
-        <v>1010</v>
+        <v>23</v>
+      </c>
+      <c r="K64" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>1206</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <f aca="false">A64+1</f>
-        <v>62</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D65" s="0" t="n">
-        <v>114</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>303</v>
-      </c>
-      <c r="F65" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="G65" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="H65" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I65" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J65" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="K65" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="L65" s="0" t="n">
-        <v>520</v>
-      </c>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <f aca="false">A65+1</f>
-        <v>63</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="0" t="n">
-        <v>116</v>
-      </c>
-      <c r="E66" s="0" t="n">
-        <v>374</v>
-      </c>
-      <c r="F66" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G66" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="H66" s="0" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="K66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L66" s="0" t="n">
-        <v>234</v>
-      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <f aca="false">A66+1</f>
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>73</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>121</v>
+        <v>266</v>
       </c>
       <c r="E67" s="0" t="n">
-        <v>358</v>
+        <v>516</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="I67" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J67" s="0" t="n">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>263</v>
+        <v>417</v>
       </c>
       <c r="L67" s="0" t="n">
-        <v>728</v>
+        <v>970</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <f aca="false">A67+1</f>
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="E68" s="0" t="n">
-        <v>330</v>
+        <v>387</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G68" s="0" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I68" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J68" s="0" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="K68" s="0" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="L68" s="0" t="n">
-        <v>810</v>
+        <v>770</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <f aca="false">A68+1</f>
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="E69" s="0" t="n">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="I69" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J69" s="0" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="K69" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L69" s="0" t="n">
-        <v>840</v>
+        <v>570</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <f aca="false">A69+1</f>
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E70" s="0" t="n">
-        <v>340</v>
+        <v>440</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H70" s="0" t="n">
-        <v>5</v>
+        <v>11.6</v>
       </c>
       <c r="I70" s="0" t="n">
         <v>2</v>
@@ -3155,369 +2964,601 @@
         <v>32</v>
       </c>
       <c r="K70" s="0" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="L70" s="0" t="n">
-        <v>520</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <f aca="false">A70+1</f>
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>209</v>
+        <v>114</v>
       </c>
       <c r="E71" s="0" t="n">
-        <v>573</v>
+        <v>303</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G71" s="0" t="n">
-        <v>33.4</v>
+        <v>7</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>8</v>
+        <v>0.2</v>
       </c>
       <c r="I71" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J71" s="0" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="K71" s="0" t="n">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="L71" s="0" t="n">
-        <v>600</v>
+        <v>520</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <f aca="false">A71+1</f>
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D72" s="0" t="n">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="E72" s="0" t="n">
-        <v>399</v>
+        <v>374</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G72" s="0" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>10.8</v>
+        <v>7.6</v>
       </c>
       <c r="I72" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="K72" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" s="0" t="n">
-        <v>601</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <f aca="false">A72+1</f>
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="E73" s="0" t="n">
-        <v>149</v>
+        <v>358</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>16.4</v>
+        <v>23</v>
       </c>
       <c r="G73" s="0" t="n">
-        <v>8.5</v>
+        <v>16</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>3.3</v>
+        <v>6.4</v>
       </c>
       <c r="I73" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J73" s="0" t="n">
-        <v>1.7</v>
+        <v>30</v>
       </c>
       <c r="K73" s="0" t="n">
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="L73" s="0" t="n">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
-        <f aca="false">A73+1</f>
-        <v>71</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D74" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="E74" s="0" t="n">
-        <v>329</v>
-      </c>
-      <c r="F74" s="0" t="n">
-        <v>25.6</v>
-      </c>
-      <c r="G74" s="0" t="n">
-        <v>20.6</v>
-      </c>
-      <c r="H74" s="0" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="I74" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J74" s="0" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="K74" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L74" s="0" t="n">
-        <v>538</v>
+        <v>728</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <f aca="false">A74+1</f>
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="E75" s="0" t="n">
-        <v>157</v>
+        <v>330</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>11.8</v>
+        <v>18</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>9.9</v>
+        <v>16</v>
       </c>
       <c r="H75" s="0" t="n">
-        <v>3.4</v>
+        <v>7</v>
       </c>
       <c r="I75" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" s="0" t="n">
-        <v>5.3</v>
+        <v>28</v>
       </c>
       <c r="K75" s="0" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="L75" s="0" t="n">
-        <v>299</v>
+        <v>810</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <f aca="false">A75+1</f>
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="E76" s="0" t="n">
-        <v>633</v>
+        <v>320</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>27.5</v>
+        <v>3</v>
       </c>
       <c r="G76" s="0" t="n">
-        <v>37.5</v>
+        <v>16</v>
       </c>
       <c r="H76" s="0" t="n">
-        <v>12.2</v>
+        <v>3</v>
       </c>
       <c r="I76" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J76" s="0" t="n">
-        <v>45.6</v>
+        <v>41</v>
       </c>
       <c r="K76" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L76" s="0" t="n">
-        <v>1168</v>
+        <v>840</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <f aca="false">A76+1</f>
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E77" s="0" t="n">
-        <v>197</v>
+        <v>340</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>2.4</v>
+        <v>14</v>
       </c>
       <c r="G77" s="0" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H77" s="0" t="n">
-        <v>2.9</v>
+        <v>5</v>
       </c>
       <c r="I77" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J77" s="0" t="n">
-        <v>15.4</v>
+        <v>32</v>
       </c>
       <c r="K77" s="0" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L77" s="0" t="n">
-        <v>78</v>
+        <v>520</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <f aca="false">A77+1</f>
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>58</v>
+        <v>209</v>
       </c>
       <c r="E78" s="0" t="n">
-        <v>190</v>
+        <v>573</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>11.5</v>
+        <v>23</v>
       </c>
       <c r="G78" s="0" t="n">
-        <v>13.3</v>
+        <v>33.4</v>
       </c>
       <c r="H78" s="0" t="n">
-        <v>5.3</v>
+        <v>8</v>
       </c>
       <c r="I78" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J78" s="0" t="n">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="K78" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L78" s="0" t="n">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
-        <f aca="false">A78+1</f>
-        <v>76</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D79" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="E79" s="0" t="n">
-        <v>257</v>
-      </c>
-      <c r="F79" s="0" t="n">
-        <v>27.1</v>
-      </c>
-      <c r="G79" s="0" t="n">
-        <v>14.1</v>
-      </c>
-      <c r="H79" s="0" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="I79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J79" s="0" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="K79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L79" s="0" t="n">
-        <v>545</v>
+        <v>600</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <f aca="false">A79+1</f>
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>142</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>399</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="0" t="n">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <f aca="false">A80+1</f>
+        <v>2</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" s="0" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <f aca="false">A81+1</f>
+        <v>3</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>329</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>20.6</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="0" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="0" t="n">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <f aca="false">A82+1</f>
+        <v>4</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="K83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" s="0" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <f aca="false">A83+1</f>
+        <v>5</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>633</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="0" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="K84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" s="0" t="n">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <f aca="false">A84+1</f>
+        <v>6</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="0" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="K85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <f aca="false">A85+1</f>
+        <v>7</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="0" t="n">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <f aca="false">A86+1</f>
+        <v>8</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="0" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="K87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="0" t="n">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <f aca="false">A87+1</f>
+        <v>9</v>
+      </c>
+      <c r="B88" s="0" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>